<commit_message>
Upgrade export function from PHPExcel to PhpSpreadsheet
</commit_message>
<xml_diff>
--- a/application/controllers/Purchases.xlsx
+++ b/application/controllers/Purchases.xlsx
@@ -4,32 +4,101 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
-  <si>
-    <t>Reference Number: TS-WF-194F-0000344_WTA</t>
-  </si>
-  <si>
-    <t>Billing Period (From): July 25,2022</t>
-  </si>
-  <si>
-    <t>Date: September 12,2022</t>
-  </si>
-  <si>
-    <t>Billing Period (To): August 25,2022</t>
-  </si>
-  <si>
-    <t>Due Date: September 25,2022</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+  <si>
+    <t>Reference Number: TS-WAC-119F4-0000037</t>
+  </si>
+  <si>
+    <t>Date: April 13,2022</t>
+  </si>
+  <si>
+    <t>Due Date: April 25,2022</t>
+  </si>
+  <si>
+    <t>Billing Period (From): April 26,2016</t>
+  </si>
+  <si>
+    <t>Billing Period (To): May 25,2016</t>
+  </si>
+  <si>
+    <t>Item No.</t>
+  </si>
+  <si>
+    <t>STL ID/TPShort Name</t>
+  </si>
+  <si>
+    <t>Billing ID</t>
+  </si>
+  <si>
+    <t>Facility Type</t>
+  </si>
+  <si>
+    <t>WHT Agent Tag</t>
+  </si>
+  <si>
+    <t>ITH Tag</t>
+  </si>
+  <si>
+    <t>Non Vatable Tag</t>
+  </si>
+  <si>
+    <t>Zero-rated Tag</t>
+  </si>
+  <si>
+    <t>Vatable Purchases</t>
+  </si>
+  <si>
+    <t>Zero Rated Purchases</t>
+  </si>
+  <si>
+    <t>Zero Rated EcoZones Purchases</t>
+  </si>
+  <si>
+    <t>Vat On Purchases</t>
+  </si>
+  <si>
+    <t>EWT</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>OR Number</t>
+  </si>
+  <si>
+    <t>Original Copy</t>
+  </si>
+  <si>
+    <t>Scanned Copy</t>
+  </si>
+  <si>
+    <t>SIPC</t>
+  </si>
+  <si>
+    <t>GEN</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>SPCPOWER</t>
   </si>
 </sst>
 </file>
@@ -37,9 +106,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -53,21 +131,47 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+  <cellXfs count="5">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -364,59 +468,224 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A5:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="25.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="15.139" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="11.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="20.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="19.852" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="37.562" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="22.28" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="8.141" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="17.567" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
       <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
+    <row r="5" spans="1:18">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
@@ -426,7 +695,7 @@
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>
@@ -435,5 +704,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>